<commit_message>
Redesign to TransactionalOperator, add continue on failure
Change doInTransaction with annotation

Change doInTransaction with annotation

Change doInTransaction with annotation

Change doInTransaction with annotation

Fix .travis.yml

Fix GlobalExceptionHandler

Add ResponseEntity and improve tests

Polish

fix GlobalExceptionHandler

fix GlobalExceptionHandler

Rename init to initRootDirectory

Small fixes

Small fixes @NotNull

Handle product duplicates

Add load_test.sh

Fix ProductToProductDtoConverter in test

Fix README.md

Reformat code

Reformat code

Zip big file

Reformat code

Disable extra tests in .travis.yml

Bump version 2.0.0
</commit_message>
<xml_diff>
--- a/src/test/resources/products1.xlsx
+++ b/src/test/resources/products1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,28 +16,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
-  <si>
-    <t>article</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Eau de Parfum</t>
   </si>
   <si>
-    <t>size</t>
+    <t>description</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>pack</t>
+  </si>
+  <si>
+    <t>art</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +75,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -153,6 +158,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -187,6 +193,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -362,18 +369,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -382,15 +389,15 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>120589</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -399,32 +406,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>120590</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>21</v>
       </c>
       <c r="D3">
         <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>1647</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>79</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -434,12 +427,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -447,12 +440,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>